<commit_message>
update bilibil spider in 12_22
</commit_message>
<xml_diff>
--- a/beautiSoupSpider/douban2.xlsx
+++ b/beautiSoupSpider/douban2.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\张霄港\Desktop\hive\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\张霄港\Desktop\hive\beautiSoupSpider\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2696,12 +2696,14 @@
   <dimension ref="A1:D251"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="232.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">

</xml_diff>